<commit_message>
updated check marks and submit button
</commit_message>
<xml_diff>
--- a/fbd-exercise/questions/sheet.xlsx
+++ b/fbd-exercise/questions/sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Question</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Click on the given reference point ( ● ), and drag out arrows to represent the various forces acting on this box sliding down an inclined plane. That is, create a Free Body Diagram. Assume there is no friction between the object and the inclined surface. Click on the SUBMIT button to check your answer.</t>
   </si>
   <si>
-    <t>1a</t>
-  </si>
-  <si>
     <t>Answer</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
     <t>Click on the NEXT button to proceed.</t>
   </si>
   <si>
-    <t>1b</t>
-  </si>
-  <si>
     <t>Drag the arrows into the box to resolve the Free Body Diagram . Click on the SUBMIT button to check your answer.</t>
   </si>
   <si>
@@ -62,9 +56,6 @@
     <t>Click on the NEXT button to proceed to the next exercise.</t>
   </si>
   <si>
-    <t>1c</t>
-  </si>
-  <si>
     <t>From the information given, which formula would you use to find the unknown (?). Select a formula and click on the SUBMIT button to check your answer.</t>
   </si>
   <si>
@@ -84,6 +75,9 @@
   </si>
   <si>
     <t>pic1</t>
+  </si>
+  <si>
+    <t>Part</t>
   </si>
 </sst>
 </file>
@@ -415,117 +409,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2</v>
-      </c>
-      <c r="H4" s="1">
-        <v>3</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>